<commit_message>
SSDM-13256: Fixing failing tests.
</commit_message>
<xml_diff>
--- a/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-sample-type-filtered-attributes-compatible-with-import.xlsx
+++ b/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-sample-type-filtered-attributes-compatible-with-import.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="33">
   <si>
     <t xml:space="preserve">SAMPLE_TYPE</t>
   </si>
@@ -40,6 +40,9 @@
     <t xml:space="preserve">Version</t>
   </si>
   <si>
+    <t xml:space="preserve">Validation script</t>
+  </si>
+  <si>
     <t xml:space="preserve">ENTRY</t>
   </si>
   <si>
@@ -50,6 +53,9 @@
   </si>
   <si>
     <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test.py</t>
   </si>
   <si>
     <t xml:space="preserve">Mandatory</t>
@@ -238,7 +244,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4:A7"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.50390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -268,27 +274,31 @@
       <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="H2" s="1"/>
-      <c r="J2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="E3" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="H3" s="1"/>
-      <c r="J3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
@@ -298,120 +308,120 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="E5" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>8</v>
-      </c>
       <c r="E6" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="K6" s="3"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J7" s="3"/>
       <c r="K7" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>